<commit_message>
pCa curves without isotypes
</commit_message>
<xml_diff>
--- a/MATLAB_code/mean_summary_pCa.xlsx
+++ b/MATLAB_code/mean_summary_pCa.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="270" uniqueCount="5">
   <si>
     <t>curve</t>
   </si>
@@ -128,13 +128,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="0">
-        <v>0.96353728821906848</v>
+        <v>1</v>
       </c>
       <c r="D3" s="0">
         <v>950</v>
       </c>
       <c r="E3" s="0">
-        <v>0.0081950779186216131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -145,13 +145,13 @@
         <v>5.2999999999999998</v>
       </c>
       <c r="C4" s="0">
-        <v>0.8610080921338723</v>
+        <v>0.92777620480442979</v>
       </c>
       <c r="D4" s="0">
         <v>950</v>
       </c>
       <c r="E4" s="0">
-        <v>0.0074784575971211745</v>
+        <v>0.072223795195570262</v>
       </c>
     </row>
     <row r="5">
@@ -162,13 +162,13 @@
         <v>5.5</v>
       </c>
       <c r="C5" s="0">
-        <v>0.58348742232183082</v>
+        <v>0.73156848902157257</v>
       </c>
       <c r="D5" s="0">
         <v>950</v>
       </c>
       <c r="E5" s="0">
-        <v>0.0045628035210848062</v>
+        <v>0.00075404922037147759</v>
       </c>
     </row>
     <row r="6">
@@ -179,13 +179,13 @@
         <v>5.7000000000000002</v>
       </c>
       <c r="C6" s="0">
-        <v>0.17525298115276425</v>
+        <v>0.44860486960559709</v>
       </c>
       <c r="D6" s="0">
         <v>950</v>
       </c>
       <c r="E6" s="0">
-        <v>0.004413970264153356</v>
+        <v>0.068412932907872953</v>
       </c>
     </row>
     <row r="7">
@@ -196,13 +196,13 @@
         <v>5.9000000000000004</v>
       </c>
       <c r="C7" s="0">
-        <v>0.0499540493904361</v>
+        <v>0.15293852533765273</v>
       </c>
       <c r="D7" s="0">
         <v>950</v>
       </c>
       <c r="E7" s="0">
-        <v>0.0021450357722000339</v>
+        <v>0.028139083648352728</v>
       </c>
     </row>
     <row r="8">
@@ -213,13 +213,13 @@
         <v>6.0999999999999996</v>
       </c>
       <c r="C8" s="0">
-        <v>0.024819042448732634</v>
+        <v>0.075637625912831158</v>
       </c>
       <c r="D8" s="0">
         <v>950</v>
       </c>
       <c r="E8" s="0">
-        <v>0.0013808150329597461</v>
+        <v>0.0283569391067643</v>
       </c>
     </row>
     <row r="9">
@@ -230,13 +230,13 @@
         <v>6.2999999999999998</v>
       </c>
       <c r="C9" s="0">
-        <v>0.013733969928802612</v>
+        <v>0.031775865014838665</v>
       </c>
       <c r="D9" s="0">
         <v>950</v>
       </c>
       <c r="E9" s="0">
-        <v>0.0007498657037436848</v>
+        <v>0.0090074153674495686</v>
       </c>
     </row>
     <row r="10">
@@ -247,13 +247,13 @@
         <v>6.5</v>
       </c>
       <c r="C10" s="0">
-        <v>0.012466309406428445</v>
+        <v>0.013374580219945247</v>
       </c>
       <c r="D10" s="0">
         <v>950</v>
       </c>
       <c r="E10" s="0">
-        <v>0.00049622970778192155</v>
+        <v>0.0049454214429347004</v>
       </c>
     </row>
     <row r="11">
@@ -264,13 +264,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="0">
-        <v>0.0052022022284200862</v>
+        <v>0.0040008204008844727</v>
       </c>
       <c r="D11" s="0">
         <v>950</v>
       </c>
       <c r="E11" s="0">
-        <v>1.8696189543931157e-05</v>
+        <v>5.132577869039652e-05</v>
       </c>
     </row>
     <row r="12">
@@ -298,13 +298,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="0">
-        <v>0.97574444962245332</v>
+        <v>1</v>
       </c>
       <c r="D13" s="0">
         <v>1150</v>
       </c>
       <c r="E13" s="0">
-        <v>0.0062174751204615167</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -315,13 +315,13 @@
         <v>5.2999999999999998</v>
       </c>
       <c r="C14" s="0">
-        <v>0.91322249464222849</v>
+        <v>1.0199387227673973</v>
       </c>
       <c r="D14" s="0">
         <v>1150</v>
       </c>
       <c r="E14" s="0">
-        <v>0.0053353941767176919</v>
+        <v>0.019938722767397277</v>
       </c>
     </row>
     <row r="15">
@@ -332,13 +332,13 @@
         <v>5.5</v>
       </c>
       <c r="C15" s="0">
-        <v>0.737122075645949</v>
+        <v>0.91365923851480035</v>
       </c>
       <c r="D15" s="0">
         <v>1150</v>
       </c>
       <c r="E15" s="0">
-        <v>0.0083449927572081268</v>
+        <v>0.015111640714474073</v>
       </c>
     </row>
     <row r="16">
@@ -349,13 +349,13 @@
         <v>5.7000000000000002</v>
       </c>
       <c r="C16" s="0">
-        <v>0.40418165783828963</v>
+        <v>0.65293828229087914</v>
       </c>
       <c r="D16" s="0">
         <v>1150</v>
       </c>
       <c r="E16" s="0">
-        <v>0.0086710624661628481</v>
+        <v>0.059831743802541915</v>
       </c>
     </row>
     <row r="17">
@@ -366,13 +366,13 @@
         <v>5.9000000000000004</v>
       </c>
       <c r="C17" s="0">
-        <v>0.12420783226517143</v>
+        <v>0.36654835753681869</v>
       </c>
       <c r="D17" s="0">
         <v>1150</v>
       </c>
       <c r="E17" s="0">
-        <v>0.0048295192568498322</v>
+        <v>0.035475837575819756</v>
       </c>
     </row>
     <row r="18">
@@ -383,13 +383,13 @@
         <v>6.0999999999999996</v>
       </c>
       <c r="C18" s="0">
-        <v>0.064720079568812525</v>
+        <v>0.14293494630484724</v>
       </c>
       <c r="D18" s="0">
         <v>1150</v>
       </c>
       <c r="E18" s="0">
-        <v>0.001481239073597516</v>
+        <v>0.026247068951715625</v>
       </c>
     </row>
     <row r="19">
@@ -400,13 +400,13 @@
         <v>6.2999999999999998</v>
       </c>
       <c r="C19" s="0">
-        <v>0.045489307080122068</v>
+        <v>0.071827198854823721</v>
       </c>
       <c r="D19" s="0">
         <v>1150</v>
       </c>
       <c r="E19" s="0">
-        <v>0.0013268531588795328</v>
+        <v>0.00037473645294306546</v>
       </c>
     </row>
     <row r="20">
@@ -417,13 +417,13 @@
         <v>6.5</v>
       </c>
       <c r="C20" s="0">
-        <v>0.040314734422869793</v>
+        <v>0.033856757712352505</v>
       </c>
       <c r="D20" s="0">
         <v>1150</v>
       </c>
       <c r="E20" s="0">
-        <v>0.00079807842639739929</v>
+        <v>0.0028455821051713518</v>
       </c>
     </row>
     <row r="21">
@@ -434,13 +434,13 @@
         <v>9</v>
       </c>
       <c r="C21" s="0">
-        <v>0.033416683407663121</v>
+        <v>0.028737813790577531</v>
       </c>
       <c r="D21" s="0">
         <v>1150</v>
       </c>
       <c r="E21" s="0">
-        <v>9.6308772109163904e-05</v>
+        <v>0.00092185323473713266</v>
       </c>
     </row>
     <row r="22">
@@ -468,13 +468,13 @@
         <v>5</v>
       </c>
       <c r="C23" s="0">
-        <v>0.9883881900115089</v>
+        <v>1</v>
       </c>
       <c r="D23" s="0">
         <v>950</v>
       </c>
       <c r="E23" s="0">
-        <v>0.01036956428938603</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -485,13 +485,13 @@
         <v>5.2999999999999998</v>
       </c>
       <c r="C24" s="0">
-        <v>0.9192828015027773</v>
+        <v>0.99721976734366358</v>
       </c>
       <c r="D24" s="0">
         <v>950</v>
       </c>
       <c r="E24" s="0">
-        <v>0.0057964759150211705</v>
+        <v>0.0027802326563364783</v>
       </c>
     </row>
     <row r="25">
@@ -502,13 +502,13 @@
         <v>5.5</v>
       </c>
       <c r="C25" s="0">
-        <v>0.73643385064199729</v>
+        <v>0.6874565028611046</v>
       </c>
       <c r="D25" s="0">
         <v>950</v>
       </c>
       <c r="E25" s="0">
-        <v>0.0046970358217444117</v>
+        <v>0.065046322737951245</v>
       </c>
     </row>
     <row r="26">
@@ -519,13 +519,13 @@
         <v>5.7000000000000002</v>
       </c>
       <c r="C26" s="0">
-        <v>0.37739183508580149</v>
+        <v>0.26608835331055697</v>
       </c>
       <c r="D26" s="0">
         <v>950</v>
       </c>
       <c r="E26" s="0">
-        <v>0.008776884220524769</v>
+        <v>0.021154206231468062</v>
       </c>
     </row>
     <row r="27">
@@ -536,13 +536,13 @@
         <v>5.9000000000000004</v>
       </c>
       <c r="C27" s="0">
-        <v>0.097150256163364035</v>
+        <v>0.089213220362641635</v>
       </c>
       <c r="D27" s="0">
         <v>950</v>
       </c>
       <c r="E27" s="0">
-        <v>0.0034662492314398883</v>
+        <v>0.027376813995345396</v>
       </c>
     </row>
     <row r="28">
@@ -553,13 +553,13 @@
         <v>6.0999999999999996</v>
       </c>
       <c r="C28" s="0">
-        <v>0.036414712392566474</v>
+        <v>0.025202537218857138</v>
       </c>
       <c r="D28" s="0">
         <v>950</v>
       </c>
       <c r="E28" s="0">
-        <v>0.001665247547018116</v>
+        <v>0.011295308279021586</v>
       </c>
     </row>
     <row r="29">
@@ -570,13 +570,13 @@
         <v>6.2999999999999998</v>
       </c>
       <c r="C29" s="0">
-        <v>0.019931002115770639</v>
+        <v>0.011182587480671271</v>
       </c>
       <c r="D29" s="0">
         <v>950</v>
       </c>
       <c r="E29" s="0">
-        <v>0.0018045214943177778</v>
+        <v>0.0032609819874478874</v>
       </c>
     </row>
     <row r="30">
@@ -587,13 +587,13 @@
         <v>6.5</v>
       </c>
       <c r="C30" s="0">
-        <v>0.010400176190631848</v>
+        <v>0.016272482841773687</v>
       </c>
       <c r="D30" s="0">
         <v>950</v>
       </c>
       <c r="E30" s="0">
-        <v>0.00070486585716830188</v>
+        <v>0.008154636712533643</v>
       </c>
     </row>
     <row r="31">
@@ -604,13 +604,13 @@
         <v>9</v>
       </c>
       <c r="C31" s="0">
-        <v>0.0039401355439621913</v>
+        <v>0.0043045535164640131</v>
       </c>
       <c r="D31" s="0">
         <v>950</v>
       </c>
       <c r="E31" s="0">
-        <v>2.3485430497941355e-05</v>
+        <v>0.00010259988803462726</v>
       </c>
     </row>
     <row r="32">
@@ -638,13 +638,13 @@
         <v>5</v>
       </c>
       <c r="C33" s="0">
-        <v>0.98889131444440037</v>
+        <v>1</v>
       </c>
       <c r="D33" s="0">
         <v>1150</v>
       </c>
       <c r="E33" s="0">
-        <v>0.0083193544264543642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -655,13 +655,13 @@
         <v>5.2999999999999998</v>
       </c>
       <c r="C34" s="0">
-        <v>0.97193282561944927</v>
+        <v>0.95869972783601165</v>
       </c>
       <c r="D34" s="0">
         <v>1150</v>
       </c>
       <c r="E34" s="0">
-        <v>0.0074409031872750562</v>
+        <v>0.041300272163988405</v>
       </c>
     </row>
     <row r="35">
@@ -672,13 +672,13 @@
         <v>5.5</v>
       </c>
       <c r="C35" s="0">
-        <v>0.91691218974920741</v>
+        <v>0.9078588854278602</v>
       </c>
       <c r="D35" s="0">
         <v>1150</v>
       </c>
       <c r="E35" s="0">
-        <v>0.0093843844425426527</v>
+        <v>0.048662646946527943</v>
       </c>
     </row>
     <row r="36">
@@ -689,13 +689,13 @@
         <v>5.7000000000000002</v>
       </c>
       <c r="C36" s="0">
-        <v>0.70093436157427258</v>
+        <v>0.56957005607573574</v>
       </c>
       <c r="D36" s="0">
         <v>1150</v>
       </c>
       <c r="E36" s="0">
-        <v>0.0088568834825232187</v>
+        <v>0.0063594554874340506</v>
       </c>
     </row>
     <row r="37">
@@ -706,13 +706,13 @@
         <v>5.9000000000000004</v>
       </c>
       <c r="C37" s="0">
-        <v>0.28067731094679577</v>
+        <v>0.23720313823263667</v>
       </c>
       <c r="D37" s="0">
         <v>1150</v>
       </c>
       <c r="E37" s="0">
-        <v>0.0043489224300677391</v>
+        <v>0.012238919802421241</v>
       </c>
     </row>
     <row r="38">
@@ -723,13 +723,13 @@
         <v>6.0999999999999996</v>
       </c>
       <c r="C38" s="0">
-        <v>0.10226607572666709</v>
+        <v>0.073704579902514791</v>
       </c>
       <c r="D38" s="0">
         <v>1150</v>
       </c>
       <c r="E38" s="0">
-        <v>0.002933472142751874</v>
+        <v>0.01480073235646898</v>
       </c>
     </row>
     <row r="39">
@@ -740,13 +740,13 @@
         <v>6.2999999999999998</v>
       </c>
       <c r="C39" s="0">
-        <v>0.056951670951469982</v>
+        <v>0.06629753361429544</v>
       </c>
       <c r="D39" s="0">
         <v>1150</v>
       </c>
       <c r="E39" s="0">
-        <v>0.00230631088137025</v>
+        <v>0.0048097104061536541</v>
       </c>
     </row>
     <row r="40">
@@ -757,13 +757,13 @@
         <v>6.5</v>
       </c>
       <c r="C40" s="0">
-        <v>0.043493737941688856</v>
+        <v>0.050795534750370137</v>
       </c>
       <c r="D40" s="0">
         <v>1150</v>
       </c>
       <c r="E40" s="0">
-        <v>0.0019692980788288358</v>
+        <v>0.0096681249227956439</v>
       </c>
     </row>
     <row r="41">
@@ -774,13 +774,13 @@
         <v>9</v>
       </c>
       <c r="C41" s="0">
-        <v>0.028467923286900815</v>
+        <v>0.02864383112886227</v>
       </c>
       <c r="D41" s="0">
         <v>1150</v>
       </c>
       <c r="E41" s="0">
-        <v>0.00019028927172290311</v>
+        <v>0.00066393072138239476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>